<commit_message>
Documentation optimization. Some fixes and clean-ups.
</commit_message>
<xml_diff>
--- a/scripts/valo-search-to-uwp-migration/input/migrate-pages.xlsx
+++ b/scripts/valo-search-to-uwp-migration/input/migrate-pages.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rueha\Source\Repos\dworld-intranet-customizations\scripts\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rueha\Source\Repos\valo-community-samples\scripts\valo-search-to-uwp-migration\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C5CB0D-69E3-4C7D-B36B-46F46DAE3BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECBBE5C-EE61-4D51-B80F-B8DCE0927150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2A68A75-3983-4725-92B4-CB7E654F6F7D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{C2A68A75-3983-4725-92B4-CB7E654F6F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Update Pages" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Site</t>
   </si>
@@ -40,18 +40,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>my-hub-prefix</t>
@@ -105,42 +93,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA29B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -160,16 +121,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BB0F8D8F-73FE-4318-8C25-12933D688273}" name="Tabelle4" displayName="Tabelle4" ref="A1:G1047927" totalsRowShown="0">
-  <autoFilter ref="A1:G1047927" xr:uid="{C86599A9-9A97-4801-A86F-32D977D0C075}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BB0F8D8F-73FE-4318-8C25-12933D688273}" name="Tabelle4" displayName="Tabelle4" ref="A1:C1047927" totalsRowShown="0">
+  <autoFilter ref="A1:C1047927" xr:uid="{C86599A9-9A97-4801-A86F-32D977D0C075}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{09D9E4EC-3BFF-4A51-8E37-45440BF0F800}" name="Hub"/>
     <tableColumn id="2" xr3:uid="{3C7CBE78-B418-4FB8-8DBB-8E039347180F}" name="Site"/>
-    <tableColumn id="3" xr3:uid="{30F5BCC0-57E5-4847-BAD8-B05FB5DF60F9}" name="Comment"/>
     <tableColumn id="4" xr3:uid="{B58F20D9-9E56-4CD1-89C9-F7834ED116D0}" name="Name"/>
-    <tableColumn id="5" xr3:uid="{62F58106-688D-4B37-9F67-D6B35A1FA722}" name="Title"/>
-    <tableColumn id="6" xr3:uid="{EA7AB17C-2154-4E84-A3EC-3D9B6A6E9DC7}" name="Template"/>
-    <tableColumn id="7" xr3:uid="{82A1B203-A8D2-4864-9260-CEFCE430FB31}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -472,24 +429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC036B2B-54D1-405B-8441-4424BBFA63DA}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="66.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="69.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -497,41 +450,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1047927">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(G1))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"ok"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2576292A-8F15-432B-BBC1-AFE059C78F5F}"/>
   </hyperlinks>

</xml_diff>